<commit_message>
Changes - Protokoll, Edit-User
</commit_message>
<xml_diff>
--- a/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Gabric.xlsx
+++ b/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Gabric.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josip\Documents\5AHWII\SWP\CCC_Projekt\Ferienspass\Taetigkeitsprotokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0AFF67-D41C-4804-926B-8B9C0FF7F90B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573F56A9-A85C-4160-8897-F386D94A1006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="882" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Datum</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>Check-Klasse programmiert, Verification von einigen Methoden und programmierten Seiten, Flipchart und Burndownchart aktualisiert, Datenbank optimiert(Probleme mit einigen Tabellen und Relationen), Programmierbeihilfe</t>
+  </si>
+  <si>
+    <t>14.01.2020</t>
+  </si>
+  <si>
+    <t>Sprintplanung (Akzeptanzkriterien, Flip Chart, Story Points,…), Start des 3. Sprints, Programmierarbeiten an Story</t>
+  </si>
+  <si>
+    <t>15.01.2020</t>
+  </si>
+  <si>
+    <t>Programmieren an Story - Admin User anzeigen, bearbeiten</t>
   </si>
 </sst>
 </file>
@@ -750,7 +762,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1026,27 +1038,47 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="26"/>
+    <row r="15" spans="1:13" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.45">
+      <c r="A15" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="24">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="D15" s="24">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>31</v>
+      </c>
       <c r="F15" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.22569444444444436</v>
       </c>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:13" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="27"/>
+      <c r="A16" s="22">
+        <v>43845</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="24">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D16" s="24">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>33</v>
+      </c>
       <c r="F16" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444531E-2</v>
       </c>
       <c r="G16" s="11"/>
     </row>
@@ -1314,7 +1346,7 @@
       <c r="E38" s="32"/>
       <c r="F38" s="21">
         <f>SUM(F7:F37)</f>
-        <v>1.4791666666666665</v>
+        <v>1.7743055555555554</v>
       </c>
       <c r="G38" s="8"/>
     </row>

</xml_diff>